<commit_message>
Added updated test cases to the Schedule Page
update to test cases, procedures and conditions
</commit_message>
<xml_diff>
--- a/Testing Spreadsheet v1.0 OrderSchedulePage.xlsx
+++ b/Testing Spreadsheet v1.0 OrderSchedulePage.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <workbookProtection workbookPassword="A6C2" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="100" windowWidth="16560" windowHeight="6350" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="105" windowWidth="16560" windowHeight="6345" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Reqs" sheetId="5" r:id="rId1"/>
@@ -195,7 +195,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="157">
   <si>
     <t xml:space="preserve">Req </t>
   </si>
@@ -405,6 +405,303 @@
   </si>
   <si>
     <t>Moderate</t>
+  </si>
+  <si>
+    <t>Tcase_1</t>
+  </si>
+  <si>
+    <t>Tcase_2</t>
+  </si>
+  <si>
+    <t>Tcase_3</t>
+  </si>
+  <si>
+    <t>Tcase_4</t>
+  </si>
+  <si>
+    <t>Tcase_5</t>
+  </si>
+  <si>
+    <t>Check 'Now' service brings user to the Order Receipt Page.</t>
+  </si>
+  <si>
+    <t>Check 'Later' service brings the user to the Order Receipt Page.</t>
+  </si>
+  <si>
+    <t>Check 'Later' service with different values.</t>
+  </si>
+  <si>
+    <t>Process certain pizza type through to the scheduling service to confirm it is accepted correctly</t>
+  </si>
+  <si>
+    <t>Check 'Now' service correctly allocates the right amount of time for the immediate pick up service.</t>
+  </si>
+  <si>
+    <t>Tcase_6</t>
+  </si>
+  <si>
+    <t>Add Classic Deluxe pizza to cart, proceed to order.</t>
+  </si>
+  <si>
+    <t>Highlight 'Now' button, click Confirm button</t>
+  </si>
+  <si>
+    <t>Schedule_Tconn_1</t>
+  </si>
+  <si>
+    <t>Steven Kennedy</t>
+  </si>
+  <si>
+    <t>Add cheese pizza to the cart, proceed to order</t>
+  </si>
+  <si>
+    <t>Tcase_7</t>
+  </si>
+  <si>
+    <t>Tcase_8</t>
+  </si>
+  <si>
+    <t>Check 'Later' service opens calendar and time selection boxes</t>
+  </si>
+  <si>
+    <t>Highlight 'Later' button</t>
+  </si>
+  <si>
+    <t>Schedule_Tconn_2</t>
+  </si>
+  <si>
+    <t>Schedule_Tconn_3</t>
+  </si>
+  <si>
+    <t>Highlight 'Later' button, click Confirm button, select 11th March '15, Hour: 18, Minute: 00</t>
+  </si>
+  <si>
+    <t>Add ….. Pizza to the cart, proceed to order</t>
+  </si>
+  <si>
+    <t>Add ….. Pizza to the cart, select …… toppings, proceed to order</t>
+  </si>
+  <si>
+    <t>Check 'Later' service allocates the right date and time as scheduled on the Order Receipt Page.</t>
+  </si>
+  <si>
+    <t>Add Meat Extravaganza Pizza to the cart, proceed to order</t>
+  </si>
+  <si>
+    <t>Highlight 'Later' button, click Confirm button, select 14th March '15, Hour: 8, Minute: 45</t>
+  </si>
+  <si>
+    <t>Schedule_Tconn_4</t>
+  </si>
+  <si>
+    <t>Highlight 'Later' button, click Confirm button, select 18 March '15, Hour: 10, Minute: 45</t>
+  </si>
+  <si>
+    <t>Schedule_Tconn_5</t>
+  </si>
+  <si>
+    <t>Check 'Later' service with different values, test should fail</t>
+  </si>
+  <si>
+    <t>Highlight 'Later' button, click Confirm button, select 19 March '15, Hour: 17, Minute: 30</t>
+  </si>
+  <si>
+    <t>Schedule_Tconn_6</t>
+  </si>
+  <si>
+    <t>Schedule_Time_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Even when a message told the user that the date entered was outside the validation for ordering within a week, the confirm button was still usable and functioned correctly. </t>
+  </si>
+  <si>
+    <t>Highlight 'Later' button, click Confirm button, select 17 March '15, Hour: 00, Minute: 00</t>
+  </si>
+  <si>
+    <t>Schedule_Tconn_7</t>
+  </si>
+  <si>
+    <t>Highlight 'Later' button, click Confirm button, select 11 March '15, Hour: 13, Minute: 15, select past time</t>
+  </si>
+  <si>
+    <t>Schedule_Time_2</t>
+  </si>
+  <si>
+    <t>Highlight 'Later' button, click Confirm button, select 15 April '15, Hour: 15, Minute: 45</t>
+  </si>
+  <si>
+    <t>Highlight 'Later' button, click Confirm button, select 18 March '15, Hour: 23, Minute: 30</t>
+  </si>
+  <si>
+    <t>Tcase_9</t>
+  </si>
+  <si>
+    <t>Tcase_10</t>
+  </si>
+  <si>
+    <t>Check 'Later' service with different values</t>
+  </si>
+  <si>
+    <t>Schedule_Time_3</t>
+  </si>
+  <si>
+    <t>Message didn't appear to prevent user from ordering outside the validation period, or the button didn't prevent the order being taken. The day was correct, but the time chosen should have been flagged by the website (i.e. 11/03/15 - 16.30; 18/03/15 - 23.30; cut-off should be at 18/03/15 - 16.30)</t>
+  </si>
+  <si>
+    <t>Requirements 4.1.31</t>
+  </si>
+  <si>
+    <t>Requirements 4.1.32</t>
+  </si>
+  <si>
+    <t>Exploratory</t>
+  </si>
+  <si>
+    <t>To check that a calendar box and selection boxes appear for the user to select the date and time for their later pizza order.</t>
+  </si>
+  <si>
+    <t>To show a logined user can order a pizza for immediate collection within a 20 minute window.</t>
+  </si>
+  <si>
+    <t>To show a logined user can order a pizza for a later collection within a period of 1 week from order.</t>
+  </si>
+  <si>
+    <t>To check the logined user can select a appriopriate date and time for a later pizza collection within the 1 week window. Checking if error messages appear or  if the order button will function when a error date/time is selected.</t>
+  </si>
+  <si>
+    <t>To show the various pizzas selected to go forward to the order schedule will actually process correctly here.</t>
+  </si>
+  <si>
+    <t>Tcase_11</t>
+  </si>
+  <si>
+    <t>Tcase_12</t>
+  </si>
+  <si>
+    <t>To check that the correct time stamp for collection appears under the Order Receipt page for the 'Now' service</t>
+  </si>
+  <si>
+    <t>To check that the correct time stamp and date for collection appears under the Order Receipt page for the 'Later' service</t>
+  </si>
+  <si>
+    <t>11/03/2015 - 17:15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Highlight 'Later' button, click Confirm button, select 18 March '15, Hour: 17, Minute: 30 </t>
+  </si>
+  <si>
+    <t>Highlight 'Later' button, click Confirm button, select 11 March '15, Hour: 18, Minute: 00</t>
+  </si>
+  <si>
+    <t>Schedule_Time_4</t>
+  </si>
+  <si>
+    <t>Validation should have picked up that the user cannot order a pizza when 45 minutes hasn't laped using the later service, as this should not have been allowed on the grounds of being too early.</t>
+  </si>
+  <si>
+    <t>Requirements 4.1.31, 4.1.33</t>
+  </si>
+  <si>
+    <t>Requirements 4.1.32, 4.1.33</t>
+  </si>
+  <si>
+    <t>Sch_Tproc_1</t>
+  </si>
+  <si>
+    <t>Sch_Tproc_2</t>
+  </si>
+  <si>
+    <t>Sch_Tproc_3</t>
+  </si>
+  <si>
+    <t>Sch_Tproc_4</t>
+  </si>
+  <si>
+    <t>Sch_Tproc_5</t>
+  </si>
+  <si>
+    <t>Sch_Tproc_6</t>
+  </si>
+  <si>
+    <t>Sch_Tproc_7</t>
+  </si>
+  <si>
+    <t>Sch_Tproc_8</t>
+  </si>
+  <si>
+    <t>Sch_Tproc_9</t>
+  </si>
+  <si>
+    <t>Sch_Tproc_10</t>
+  </si>
+  <si>
+    <t>Sch_Tproc_11</t>
+  </si>
+  <si>
+    <t>Sch_Tproc_12</t>
+  </si>
+  <si>
+    <t>Carried out by Test Inspector</t>
+  </si>
+  <si>
+    <t>Automated Selenium Test</t>
+  </si>
+  <si>
+    <t>Order complete. Order Receipt Page appears</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Calendar box, Selection boxes for Hour and Minute appear </t>
+  </si>
+  <si>
+    <t>Under the order schedule section, the now collection service is clicked and the confirm button pressed to complete the order</t>
+  </si>
+  <si>
+    <t>Under the order schedule section, click the later button</t>
+  </si>
+  <si>
+    <t>Within the Later service under the order schedule section, set values for a mid-week collection from order date</t>
+  </si>
+  <si>
+    <t>Within the Later service under the order schedule section, set values for same day collection and later in the evening</t>
+  </si>
+  <si>
+    <t>Within the Later service under the order schedule section, set values for late week collection on the last available day to do so</t>
+  </si>
+  <si>
+    <t>Sch_Tproc_13</t>
+  </si>
+  <si>
+    <t>Denied order. Order will have to be re-scheduled for a appriopriate time</t>
+  </si>
+  <si>
+    <t>Within the Later service under the order schedule section, set values outside of the allocated week period for ordering</t>
+  </si>
+  <si>
+    <t>Within the Later service under the order schedule section, set values for midnight of a certain day within the week</t>
+  </si>
+  <si>
+    <t>Within the Later service under the order schedule section, set values of the time two hours ahead the same day as ordering</t>
+  </si>
+  <si>
+    <t>Within the Later service under the order schedule section, set values of the month of ordering to 1 month ahead of the current month</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Within the Later service under the order schedule section, set values that the order is on the last available day to order and at a time outside the total week hours boundary </t>
+  </si>
+  <si>
+    <t>Within the Later service under the order schedule section, set values so that the order is just outside the 45 minute period of ordering too early</t>
+  </si>
+  <si>
+    <t>Within the Later service under the order schedule section, set values so that the order is inside the 45 minute period of ordering too early</t>
+  </si>
+  <si>
+    <t>Tcase_13</t>
+  </si>
+  <si>
+    <t>Highlight 'Later' button, click Confirm button, select 21 February '15, Hour: 14, Minute: 00</t>
+  </si>
+  <si>
+    <t>Within the Later service under the order schedule section, set values for a order that is 1 month back from the current month</t>
   </si>
 </sst>
 </file>
@@ -591,7 +888,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -677,6 +974,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -736,7 +1036,6 @@
           <c:dLbls>
             <c:dLbl>
               <c:idx val="0"/>
-              <c:layout/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
               <c:showCatName val="0"/>
@@ -746,7 +1045,6 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="1"/>
-              <c:layout/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
               <c:showCatName val="0"/>
@@ -756,7 +1054,6 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="2"/>
-              <c:layout/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
               <c:showCatName val="0"/>
@@ -773,7 +1070,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Test Cases'!$T$8:$T$10</c:f>
+              <c:f>'Test Cases'!$T$26:$T$28</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -790,15 +1087,15 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Test Cases'!$U$8:$U$10</c:f>
+              <c:f>'Test Cases'!$U$26:$U$28</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -821,7 +1118,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -863,7 +1159,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Test Cases'!$T$26:$T$30</c:f>
+              <c:f>'Test Cases'!$T$44:$T$48</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -886,7 +1182,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Test Cases'!$U$26:$U$30</c:f>
+              <c:f>'Test Cases'!$U$44:$U$48</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -900,7 +1196,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -918,11 +1214,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="50486272"/>
-        <c:axId val="50496640"/>
+        <c:axId val="41196544"/>
+        <c:axId val="41218816"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="50486272"/>
+        <c:axId val="41196544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -931,7 +1227,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50496640"/>
+        <c:crossAx val="41218816"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -939,7 +1235,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="50496640"/>
+        <c:axId val="41218816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -950,7 +1246,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50486272"/>
+        <c:crossAx val="41196544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -973,13 +1269,13 @@
     <xdr:from>
       <xdr:col>22</xdr:col>
       <xdr:colOff>46567</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:row>24</xdr:row>
       <xdr:rowOff>16933</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>29</xdr:col>
       <xdr:colOff>351367</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>37</xdr:row>
       <xdr:rowOff>169333</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1003,13 +1299,13 @@
     <xdr:from>
       <xdr:col>22</xdr:col>
       <xdr:colOff>21166</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:row>41</xdr:row>
       <xdr:rowOff>16933</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>29</xdr:col>
       <xdr:colOff>325966</xdr:colOff>
-      <xdr:row>37</xdr:row>
+      <xdr:row>55</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1325,9 +1621,9 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.54296875" customWidth="1"/>
+    <col min="1" max="1" width="17.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
@@ -1359,17 +1655,17 @@
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.6328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="47.81640625" customWidth="1"/>
-    <col min="3" max="3" width="15.6328125" customWidth="1"/>
+    <col min="1" max="1" width="21.140625" customWidth="1"/>
+    <col min="2" max="2" width="47.85546875" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="29" t="s">
         <v>3</v>
       </c>
@@ -1383,95 +1679,151 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="35.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
+    <row r="2" spans="1:9" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="H2" s="5" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="35.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
+    <row r="3" spans="1:9" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="H3" s="5"/>
     </row>
-    <row r="4" spans="1:9" ht="23.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
+    <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="H4" s="6" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="23.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
+    <row r="5" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="A5" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="H5" s="6" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="23.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
+    <row r="6" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="H6" s="6" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="23.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
+    <row r="7" spans="1:9" ht="45" x14ac:dyDescent="0.35">
+      <c r="A7" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="H7" s="7" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="23.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
+    <row r="8" spans="1:9" ht="45" x14ac:dyDescent="0.35">
+      <c r="A8" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="I8" s="8" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A9" s="1"/>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="11"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A10" s="1"/>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="11"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A11" s="1"/>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="11"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
       <c r="D13" s="1"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
       <c r="D14" s="1"/>
     </row>
   </sheetData>
@@ -1497,32 +1849,32 @@
   <sheetPr>
     <tabColor theme="9" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:Z161"/>
+  <dimension ref="A1:Z179"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="P11" sqref="P11"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.1796875" customWidth="1"/>
-    <col min="2" max="2" width="24.90625" customWidth="1"/>
-    <col min="3" max="3" width="23.08984375" customWidth="1"/>
-    <col min="4" max="4" width="32.453125" customWidth="1"/>
-    <col min="5" max="6" width="18.54296875" customWidth="1"/>
-    <col min="7" max="7" width="22.6328125" customWidth="1"/>
+    <col min="1" max="1" width="16.140625" customWidth="1"/>
+    <col min="2" max="2" width="24.85546875" customWidth="1"/>
+    <col min="3" max="3" width="23.140625" customWidth="1"/>
+    <col min="4" max="4" width="32.42578125" customWidth="1"/>
+    <col min="5" max="6" width="18.5703125" customWidth="1"/>
+    <col min="7" max="7" width="22.5703125" customWidth="1"/>
     <col min="8" max="8" width="13" customWidth="1"/>
-    <col min="9" max="9" width="18.08984375" customWidth="1"/>
-    <col min="10" max="10" width="23.6328125" customWidth="1"/>
-    <col min="12" max="12" width="11.54296875" customWidth="1"/>
-    <col min="13" max="13" width="12.81640625" customWidth="1"/>
-    <col min="14" max="14" width="11.7265625" customWidth="1"/>
-    <col min="15" max="15" width="41.81640625" customWidth="1"/>
-    <col min="16" max="16" width="16.7265625" customWidth="1"/>
-    <col min="20" max="20" width="13.90625" customWidth="1"/>
+    <col min="9" max="9" width="18.140625" customWidth="1"/>
+    <col min="10" max="10" width="23.5703125" customWidth="1"/>
+    <col min="12" max="12" width="11.5703125" customWidth="1"/>
+    <col min="13" max="13" width="12.85546875" customWidth="1"/>
+    <col min="14" max="14" width="11.7109375" customWidth="1"/>
+    <col min="15" max="15" width="41.85546875" customWidth="1"/>
+    <col min="16" max="16" width="16.7109375" customWidth="1"/>
+    <col min="20" max="20" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="28" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:26" ht="27.95" x14ac:dyDescent="0.35">
       <c r="A1" s="15" t="s">
         <v>7</v>
       </c>
@@ -1570,16 +1922,34 @@
       </c>
       <c r="P1" s="20"/>
     </row>
-    <row r="2" spans="1:26" ht="23.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="12"/>
+    <row r="2" spans="1:26" ht="42.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="13">
+        <v>42074</v>
+      </c>
+      <c r="H2" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="I2" s="12" t="s">
+        <v>72</v>
+      </c>
       <c r="J2" s="3"/>
       <c r="K2" s="4"/>
       <c r="L2" s="4"/>
@@ -1591,15 +1961,34 @@
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="23.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="27"/>
+    <row r="3" spans="1:26" ht="42.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="G3" s="13">
+        <v>42074</v>
+      </c>
+      <c r="H3" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="I3" s="12" t="s">
+        <v>72</v>
+      </c>
       <c r="J3" s="3"/>
       <c r="K3" s="4"/>
       <c r="L3" s="4"/>
@@ -1607,457 +1996,801 @@
       <c r="N3" s="3"/>
       <c r="O3" s="9"/>
       <c r="P3" s="10"/>
-      <c r="T3" s="28" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="4" spans="1:26" ht="23.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="27"/>
-      <c r="I4" s="14"/>
-      <c r="J4" s="9"/>
+      <c r="S3" s="5"/>
+    </row>
+    <row r="4" spans="1:26" ht="42.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" s="13">
+        <v>42074</v>
+      </c>
+      <c r="H4" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="I4" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="J4" s="3"/>
       <c r="K4" s="4"/>
       <c r="L4" s="4"/>
-      <c r="M4" s="9"/>
-      <c r="N4" s="9"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
       <c r="O4" s="9"/>
       <c r="P4" s="10"/>
-      <c r="Z4" s="5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="27"/>
-      <c r="I5" s="14"/>
-      <c r="J5" s="9"/>
+      <c r="T4" s="28" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" ht="42.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="G5" s="13">
+        <v>42074</v>
+      </c>
+      <c r="H5" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="I5" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="J5" s="3"/>
       <c r="K5" s="4"/>
       <c r="L5" s="4"/>
-      <c r="M5" s="9"/>
-      <c r="N5" s="9"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
       <c r="O5" s="9"/>
       <c r="P5" s="10"/>
-    </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="27"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="9"/>
+      <c r="T5" s="28"/>
+    </row>
+    <row r="6" spans="1:26" ht="42.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="G6" s="13">
+        <v>42074</v>
+      </c>
+      <c r="H6" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="I6" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="J6" s="3"/>
       <c r="K6" s="4"/>
       <c r="L6" s="4"/>
-      <c r="M6" s="9"/>
-      <c r="N6" s="9"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
       <c r="O6" s="9"/>
       <c r="P6" s="10"/>
-    </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="27"/>
-      <c r="I7" s="14"/>
-      <c r="J7" s="9"/>
-      <c r="K7" s="4"/>
-      <c r="L7" s="4"/>
-      <c r="M7" s="9"/>
-      <c r="N7" s="9"/>
-      <c r="O7" s="9"/>
+      <c r="T6" s="28"/>
+    </row>
+    <row r="7" spans="1:26" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="G7" s="13">
+        <v>42074</v>
+      </c>
+      <c r="H7" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="I7" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="K7" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="L7" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="M7" s="13">
+        <v>42074</v>
+      </c>
+      <c r="N7" s="3"/>
+      <c r="O7" s="3" t="s">
+        <v>93</v>
+      </c>
       <c r="P7" s="10"/>
-      <c r="T7" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="27"/>
-      <c r="I8" s="10"/>
-      <c r="J8" s="10"/>
+      <c r="T7" s="28"/>
+    </row>
+    <row r="8" spans="1:26" ht="42.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="G8" s="13">
+        <v>42074</v>
+      </c>
+      <c r="H8" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="I8" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="J8" s="3"/>
       <c r="K8" s="4"/>
-      <c r="L8" s="10"/>
-      <c r="M8" s="10"/>
-      <c r="N8" s="10"/>
-      <c r="O8" s="10"/>
+      <c r="L8" s="4"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="3"/>
+      <c r="O8" s="9"/>
       <c r="P8" s="10"/>
-      <c r="T8" t="s">
-        <v>53</v>
-      </c>
-      <c r="U8" s="32">
-        <f>COUNTIF(H2:H90,"*Passed*")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="27"/>
-      <c r="I9" s="10"/>
-      <c r="J9" s="10"/>
+      <c r="T8" s="28"/>
+    </row>
+    <row r="9" spans="1:26" ht="57" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="G9" s="13">
+        <v>42074</v>
+      </c>
+      <c r="H9" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="I9" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="J9" s="3"/>
       <c r="K9" s="4"/>
-      <c r="L9" s="10"/>
-      <c r="M9" s="10"/>
-      <c r="N9" s="10"/>
-      <c r="O9" s="10"/>
+      <c r="L9" s="4"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
+      <c r="O9" s="9"/>
       <c r="P9" s="10"/>
-      <c r="T9" t="s">
+      <c r="T9" s="28"/>
+    </row>
+    <row r="10" spans="1:26" ht="71.25" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="G10" s="13">
+        <v>42074</v>
+      </c>
+      <c r="H10" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="U9" s="32">
-        <f>COUNTIF(H3:H90,"*Failed*")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="E10" s="10"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="27"/>
-      <c r="I10" s="10"/>
-      <c r="J10" s="10"/>
-      <c r="K10" s="4"/>
-      <c r="L10" s="10"/>
-      <c r="M10" s="10"/>
-      <c r="N10" s="10"/>
-      <c r="O10" s="10"/>
+      <c r="I10" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="K10" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="L10" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="M10" s="13">
+        <v>42074</v>
+      </c>
+      <c r="N10" s="3"/>
+      <c r="O10" s="3" t="s">
+        <v>93</v>
+      </c>
       <c r="P10" s="10"/>
-      <c r="T10" t="s">
-        <v>54</v>
-      </c>
-      <c r="U10" s="32">
-        <f>COUNTIF(H4:H90,"*Not*")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="E11" s="10"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="27"/>
-      <c r="I11" s="10"/>
-      <c r="J11" s="10"/>
-      <c r="K11" s="4"/>
-      <c r="L11" s="10"/>
-      <c r="M11" s="10"/>
-      <c r="N11" s="10"/>
-      <c r="O11" s="10"/>
+      <c r="T10" s="28"/>
+    </row>
+    <row r="11" spans="1:26" ht="114" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="G11" s="13">
+        <v>42074</v>
+      </c>
+      <c r="H11" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="I11" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="K11" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="L11" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="M11" s="13">
+        <v>42074</v>
+      </c>
+      <c r="N11" s="3"/>
+      <c r="O11" s="3" t="s">
+        <v>104</v>
+      </c>
       <c r="P11" s="10"/>
-    </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="E12" s="10"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="27"/>
-      <c r="I12" s="10"/>
-      <c r="J12" s="10"/>
-      <c r="K12" s="10"/>
-      <c r="L12" s="10"/>
-      <c r="M12" s="10"/>
-      <c r="N12" s="10"/>
-      <c r="O12" s="10"/>
+      <c r="Z11" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" ht="42.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="G12" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="H12" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="I12" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="J12" s="3"/>
+      <c r="K12" s="4"/>
+      <c r="L12" s="4"/>
+      <c r="M12" s="13"/>
+      <c r="N12" s="3"/>
+      <c r="O12" s="3"/>
       <c r="P12" s="10"/>
-    </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="E13" s="10"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="27"/>
-      <c r="I13" s="10"/>
-      <c r="J13" s="10"/>
-      <c r="K13" s="10"/>
-      <c r="L13" s="10"/>
-      <c r="M13" s="10"/>
-      <c r="N13" s="10"/>
-      <c r="O13" s="10"/>
+      <c r="Z12" s="5"/>
+    </row>
+    <row r="13" spans="1:26" ht="71.25" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="G13" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="H13" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="I13" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="K13" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="L13" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="M13" s="13">
+        <v>42074</v>
+      </c>
+      <c r="N13" s="3"/>
+      <c r="O13" s="3" t="s">
+        <v>121</v>
+      </c>
       <c r="P13" s="10"/>
-    </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="E14" s="10"/>
-      <c r="F14" s="11"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="27"/>
-      <c r="I14" s="10"/>
-      <c r="J14" s="10"/>
-      <c r="K14" s="10"/>
-      <c r="L14" s="10"/>
-      <c r="M14" s="10"/>
-      <c r="N14" s="10"/>
-      <c r="O14" s="10"/>
+      <c r="Z13" s="5"/>
+    </row>
+    <row r="14" spans="1:26" ht="57" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="F14" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="G14" s="13">
+        <v>42074</v>
+      </c>
+      <c r="H14" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="I14" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="J14" s="3"/>
+      <c r="K14" s="4"/>
+      <c r="L14" s="4"/>
+      <c r="M14" s="13"/>
+      <c r="N14" s="3"/>
+      <c r="O14" s="3"/>
       <c r="P14" s="10"/>
-    </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="E15" s="10"/>
+      <c r="Z14" s="5"/>
+    </row>
+    <row r="15" spans="1:26" ht="71.25" x14ac:dyDescent="0.25">
+      <c r="A15" s="3"/>
+      <c r="B15" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D15" s="3"/>
+      <c r="E15" s="11" t="s">
+        <v>88</v>
+      </c>
       <c r="F15" s="11"/>
-      <c r="G15" s="10"/>
+      <c r="G15" s="12"/>
       <c r="H15" s="27"/>
-      <c r="I15" s="10"/>
-      <c r="J15" s="10"/>
-      <c r="K15" s="10"/>
-      <c r="L15" s="10"/>
-      <c r="M15" s="10"/>
-      <c r="N15" s="10"/>
-      <c r="O15" s="10"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="9"/>
+      <c r="K15" s="4"/>
+      <c r="L15" s="4"/>
+      <c r="M15" s="9"/>
+      <c r="N15" s="9"/>
+      <c r="O15" s="9"/>
       <c r="P15" s="10"/>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="E16" s="10"/>
+    <row r="16" spans="1:26" ht="71.25" x14ac:dyDescent="0.25">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="11" t="s">
+        <v>88</v>
+      </c>
       <c r="F16" s="11"/>
-      <c r="G16" s="10"/>
+      <c r="G16" s="12"/>
       <c r="H16" s="27"/>
-      <c r="I16" s="10"/>
-      <c r="J16" s="10"/>
-      <c r="K16" s="10"/>
-      <c r="L16" s="10"/>
-      <c r="M16" s="10"/>
-      <c r="N16" s="10"/>
-      <c r="O16" s="10"/>
+      <c r="I16" s="14"/>
+      <c r="J16" s="9"/>
+      <c r="K16" s="4"/>
+      <c r="L16" s="4"/>
+      <c r="M16" s="9"/>
+      <c r="N16" s="9"/>
+      <c r="O16" s="9"/>
       <c r="P16" s="10"/>
     </row>
-    <row r="17" spans="5:21" x14ac:dyDescent="0.35">
-      <c r="E17" s="10"/>
+    <row r="17" spans="1:21" ht="71.25" x14ac:dyDescent="0.25">
+      <c r="A17" s="3"/>
+      <c r="B17" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="11" t="s">
+        <v>88</v>
+      </c>
       <c r="F17" s="11"/>
-      <c r="G17" s="10"/>
+      <c r="G17" s="12"/>
       <c r="H17" s="27"/>
-      <c r="I17" s="10"/>
-      <c r="J17" s="10"/>
-      <c r="K17" s="10"/>
-      <c r="L17" s="10"/>
-      <c r="M17" s="10"/>
-      <c r="N17" s="10"/>
-      <c r="O17" s="10"/>
+      <c r="I17" s="14"/>
+      <c r="J17" s="9"/>
+      <c r="K17" s="4"/>
+      <c r="L17" s="4"/>
+      <c r="M17" s="9"/>
+      <c r="N17" s="9"/>
+      <c r="O17" s="9"/>
       <c r="P17" s="10"/>
     </row>
-    <row r="18" spans="5:21" x14ac:dyDescent="0.35">
-      <c r="E18" s="10"/>
+    <row r="18" spans="1:21" ht="71.25" x14ac:dyDescent="0.25">
+      <c r="A18" s="3"/>
+      <c r="B18" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="11" t="s">
+        <v>88</v>
+      </c>
       <c r="F18" s="11"/>
-      <c r="G18" s="10"/>
+      <c r="G18" s="12"/>
       <c r="H18" s="27"/>
-      <c r="I18" s="10"/>
-      <c r="J18" s="10"/>
-      <c r="K18" s="10"/>
-      <c r="L18" s="10"/>
-      <c r="M18" s="10"/>
-      <c r="N18" s="10"/>
-      <c r="O18" s="10"/>
+      <c r="I18" s="14"/>
+      <c r="J18" s="9"/>
+      <c r="K18" s="4"/>
+      <c r="L18" s="4"/>
+      <c r="M18" s="9"/>
+      <c r="N18" s="9"/>
+      <c r="O18" s="9"/>
       <c r="P18" s="10"/>
     </row>
-    <row r="19" spans="5:21" x14ac:dyDescent="0.35">
-      <c r="E19" s="10"/>
+    <row r="19" spans="1:21" ht="71.25" x14ac:dyDescent="0.25">
+      <c r="A19" s="3"/>
+      <c r="B19" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D19" s="3"/>
+      <c r="E19" s="11" t="s">
+        <v>88</v>
+      </c>
       <c r="F19" s="11"/>
-      <c r="G19" s="10"/>
+      <c r="G19" s="12"/>
       <c r="H19" s="27"/>
-      <c r="I19" s="10"/>
-      <c r="J19" s="10"/>
-      <c r="K19" s="10"/>
-      <c r="L19" s="10"/>
-      <c r="M19" s="10"/>
-      <c r="N19" s="10"/>
-      <c r="O19" s="10"/>
+      <c r="I19" s="14"/>
+      <c r="J19" s="9"/>
+      <c r="K19" s="4"/>
+      <c r="L19" s="4"/>
+      <c r="M19" s="9"/>
+      <c r="N19" s="9"/>
+      <c r="O19" s="9"/>
       <c r="P19" s="10"/>
     </row>
-    <row r="20" spans="5:21" x14ac:dyDescent="0.35">
-      <c r="E20" s="10"/>
+    <row r="20" spans="1:21" ht="71.25" x14ac:dyDescent="0.25">
+      <c r="A20" s="3"/>
+      <c r="B20" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="11" t="s">
+        <v>88</v>
+      </c>
       <c r="F20" s="11"/>
-      <c r="G20" s="10"/>
+      <c r="G20" s="12"/>
       <c r="H20" s="27"/>
-      <c r="I20" s="10"/>
-      <c r="J20" s="10"/>
-      <c r="K20" s="10"/>
-      <c r="L20" s="10"/>
-      <c r="M20" s="10"/>
-      <c r="N20" s="10"/>
-      <c r="O20" s="10"/>
+      <c r="I20" s="14"/>
+      <c r="J20" s="9"/>
+      <c r="K20" s="4"/>
+      <c r="L20" s="4"/>
+      <c r="M20" s="9"/>
+      <c r="N20" s="9"/>
+      <c r="O20" s="9"/>
       <c r="P20" s="10"/>
     </row>
-    <row r="21" spans="5:21" x14ac:dyDescent="0.35">
-      <c r="E21" s="10"/>
+    <row r="21" spans="1:21" ht="71.25" x14ac:dyDescent="0.25">
+      <c r="A21" s="3"/>
+      <c r="B21" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="11" t="s">
+        <v>88</v>
+      </c>
       <c r="F21" s="11"/>
-      <c r="G21" s="10"/>
+      <c r="G21" s="12"/>
       <c r="H21" s="27"/>
-      <c r="I21" s="10"/>
-      <c r="J21" s="10"/>
-      <c r="K21" s="10"/>
-      <c r="L21" s="10"/>
-      <c r="M21" s="10"/>
-      <c r="N21" s="10"/>
-      <c r="O21" s="10"/>
+      <c r="I21" s="14"/>
+      <c r="J21" s="9"/>
+      <c r="K21" s="4"/>
+      <c r="L21" s="4"/>
+      <c r="M21" s="9"/>
+      <c r="N21" s="9"/>
+      <c r="O21" s="9"/>
       <c r="P21" s="10"/>
     </row>
-    <row r="22" spans="5:21" x14ac:dyDescent="0.35">
-      <c r="E22" s="10"/>
+    <row r="22" spans="1:21" ht="71.25" x14ac:dyDescent="0.25">
+      <c r="A22" s="3"/>
+      <c r="B22" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="11" t="s">
+        <v>88</v>
+      </c>
       <c r="F22" s="11"/>
-      <c r="G22" s="10"/>
+      <c r="G22" s="12"/>
       <c r="H22" s="27"/>
-      <c r="I22" s="10"/>
-      <c r="J22" s="10"/>
-      <c r="K22" s="10"/>
-      <c r="L22" s="10"/>
-      <c r="M22" s="10"/>
-      <c r="N22" s="10"/>
-      <c r="O22" s="10"/>
+      <c r="I22" s="14"/>
+      <c r="J22" s="9"/>
+      <c r="K22" s="4"/>
+      <c r="L22" s="4"/>
+      <c r="M22" s="9"/>
+      <c r="N22" s="9"/>
+      <c r="O22" s="9"/>
       <c r="P22" s="10"/>
     </row>
-    <row r="23" spans="5:21" x14ac:dyDescent="0.35">
-      <c r="E23" s="10"/>
+    <row r="23" spans="1:21" ht="71.25" x14ac:dyDescent="0.25">
+      <c r="A23" s="3"/>
+      <c r="B23" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="11" t="s">
+        <v>88</v>
+      </c>
       <c r="F23" s="11"/>
-      <c r="G23" s="10"/>
+      <c r="G23" s="12"/>
       <c r="H23" s="27"/>
-      <c r="I23" s="10"/>
-      <c r="J23" s="10"/>
-      <c r="K23" s="10"/>
-      <c r="L23" s="10"/>
-      <c r="M23" s="10"/>
-      <c r="N23" s="10"/>
-      <c r="O23" s="10"/>
+      <c r="I23" s="14"/>
+      <c r="J23" s="9"/>
+      <c r="K23" s="4"/>
+      <c r="L23" s="4"/>
+      <c r="M23" s="9"/>
+      <c r="N23" s="9"/>
+      <c r="O23" s="9"/>
       <c r="P23" s="10"/>
     </row>
-    <row r="24" spans="5:21" x14ac:dyDescent="0.35">
-      <c r="E24" s="10"/>
+    <row r="24" spans="1:21" ht="71.25" x14ac:dyDescent="0.25">
+      <c r="A24" s="3"/>
+      <c r="B24" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="D24" s="3"/>
+      <c r="E24" s="11" t="s">
+        <v>91</v>
+      </c>
       <c r="F24" s="11"/>
-      <c r="G24" s="10"/>
+      <c r="G24" s="12"/>
       <c r="H24" s="27"/>
-      <c r="I24" s="10"/>
-      <c r="J24" s="10"/>
-      <c r="K24" s="10"/>
-      <c r="L24" s="10"/>
-      <c r="M24" s="10"/>
-      <c r="N24" s="10"/>
-      <c r="O24" s="10"/>
+      <c r="I24" s="14"/>
+      <c r="J24" s="9"/>
+      <c r="K24" s="4"/>
+      <c r="L24" s="4"/>
+      <c r="M24" s="9"/>
+      <c r="N24" s="9"/>
+      <c r="O24" s="9"/>
       <c r="P24" s="10"/>
     </row>
-    <row r="25" spans="5:21" x14ac:dyDescent="0.35">
-      <c r="E25" s="10"/>
+    <row r="25" spans="1:21" ht="71.25" x14ac:dyDescent="0.25">
+      <c r="A25" s="3"/>
+      <c r="B25" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="D25" s="3"/>
+      <c r="E25" s="11" t="s">
+        <v>95</v>
+      </c>
       <c r="F25" s="11"/>
-      <c r="G25" s="10"/>
+      <c r="G25" s="13"/>
       <c r="H25" s="27"/>
-      <c r="I25" s="10"/>
-      <c r="J25" s="10"/>
-      <c r="K25" s="10"/>
-      <c r="L25" s="10"/>
-      <c r="M25" s="10"/>
-      <c r="N25" s="10"/>
-      <c r="O25" s="10"/>
+      <c r="I25" s="14"/>
+      <c r="J25" s="9"/>
+      <c r="K25" s="4"/>
+      <c r="L25" s="4"/>
+      <c r="M25" s="9"/>
+      <c r="N25" s="9"/>
+      <c r="O25" s="9"/>
       <c r="P25" s="10"/>
       <c r="T25" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="26" spans="5:21" x14ac:dyDescent="0.35">
-      <c r="E26" s="10"/>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A26" s="1"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
       <c r="F26" s="11"/>
-      <c r="G26" s="10"/>
+      <c r="G26" s="1"/>
       <c r="H26" s="27"/>
       <c r="I26" s="10"/>
       <c r="J26" s="10"/>
-      <c r="K26" s="10"/>
+      <c r="K26" s="4"/>
       <c r="L26" s="10"/>
       <c r="M26" s="10"/>
       <c r="N26" s="10"/>
       <c r="O26" s="10"/>
       <c r="P26" s="10"/>
       <c r="T26" t="s">
-        <v>34</v>
+        <v>53</v>
       </c>
       <c r="U26" s="32">
-        <f>COUNTIF(L2:L50,"*Minor*")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="5:21" x14ac:dyDescent="0.35">
-      <c r="E27" s="10"/>
+        <f>COUNTIF(H2:H108,"*Passed*")</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A27" s="1"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
       <c r="F27" s="11"/>
-      <c r="G27" s="10"/>
+      <c r="G27" s="1"/>
       <c r="H27" s="27"/>
       <c r="I27" s="10"/>
       <c r="J27" s="10"/>
-      <c r="K27" s="10"/>
+      <c r="K27" s="4"/>
       <c r="L27" s="10"/>
       <c r="M27" s="10"/>
       <c r="N27" s="10"/>
       <c r="O27" s="10"/>
       <c r="P27" s="10"/>
       <c r="T27" t="s">
-        <v>57</v>
+        <v>25</v>
       </c>
       <c r="U27" s="32">
-        <f>COUNTIF(L2:L7,"*Moderate*")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="5:21" x14ac:dyDescent="0.35">
+        <f>COUNTIF(H4:H108,"*Failed*")</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B28" s="3"/>
       <c r="E28" s="10"/>
       <c r="F28" s="11"/>
       <c r="G28" s="10"/>
       <c r="H28" s="27"/>
       <c r="I28" s="10"/>
       <c r="J28" s="10"/>
-      <c r="K28" s="10"/>
+      <c r="K28" s="4"/>
       <c r="L28" s="10"/>
       <c r="M28" s="10"/>
       <c r="N28" s="10"/>
       <c r="O28" s="10"/>
       <c r="P28" s="10"/>
       <c r="T28" t="s">
-        <v>35</v>
+        <v>54</v>
       </c>
       <c r="U28" s="32">
-        <f>COUNTIF(L2:L7,"*Major*")</f>
+        <f>COUNTIF(H11:H108,"*Not*")</f>
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="5:21" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B29" s="3"/>
       <c r="E29" s="10"/>
       <c r="F29" s="11"/>
       <c r="G29" s="10"/>
       <c r="H29" s="27"/>
       <c r="I29" s="10"/>
       <c r="J29" s="10"/>
-      <c r="K29" s="10"/>
+      <c r="K29" s="4"/>
       <c r="L29" s="10"/>
       <c r="M29" s="10"/>
       <c r="N29" s="10"/>
       <c r="O29" s="10"/>
       <c r="P29" s="10"/>
-      <c r="T29" t="s">
-        <v>36</v>
-      </c>
-      <c r="U29" s="32">
-        <f>COUNTIF(L2:L7,"*Critical*")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="5:21" x14ac:dyDescent="0.35">
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B30" s="3"/>
       <c r="E30" s="10"/>
       <c r="F30" s="11"/>
       <c r="G30" s="10"/>
@@ -2070,15 +2803,9 @@
       <c r="N30" s="10"/>
       <c r="O30" s="10"/>
       <c r="P30" s="10"/>
-      <c r="T30" t="s">
-        <v>38</v>
-      </c>
-      <c r="U30" s="32">
-        <f>COUNTIF(L2:L7,"*Cometic*")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="5:21" x14ac:dyDescent="0.35">
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B31" s="3"/>
       <c r="E31" s="10"/>
       <c r="F31" s="11"/>
       <c r="G31" s="10"/>
@@ -2092,7 +2819,8 @@
       <c r="O31" s="10"/>
       <c r="P31" s="10"/>
     </row>
-    <row r="32" spans="5:21" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B32" s="3"/>
       <c r="E32" s="10"/>
       <c r="F32" s="11"/>
       <c r="G32" s="10"/>
@@ -2106,7 +2834,8 @@
       <c r="O32" s="10"/>
       <c r="P32" s="10"/>
     </row>
-    <row r="33" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B33" s="3"/>
       <c r="E33" s="10"/>
       <c r="F33" s="11"/>
       <c r="G33" s="10"/>
@@ -2120,7 +2849,8 @@
       <c r="O33" s="10"/>
       <c r="P33" s="10"/>
     </row>
-    <row r="34" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B34" s="3"/>
       <c r="E34" s="10"/>
       <c r="F34" s="11"/>
       <c r="G34" s="10"/>
@@ -2134,7 +2864,8 @@
       <c r="O34" s="10"/>
       <c r="P34" s="10"/>
     </row>
-    <row r="35" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B35" s="3"/>
       <c r="E35" s="10"/>
       <c r="F35" s="11"/>
       <c r="G35" s="10"/>
@@ -2148,7 +2879,8 @@
       <c r="O35" s="10"/>
       <c r="P35" s="10"/>
     </row>
-    <row r="36" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B36" s="3"/>
       <c r="E36" s="10"/>
       <c r="F36" s="11"/>
       <c r="G36" s="10"/>
@@ -2162,7 +2894,7 @@
       <c r="O36" s="10"/>
       <c r="P36" s="10"/>
     </row>
-    <row r="37" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:21" ht="14.45" x14ac:dyDescent="0.35">
       <c r="E37" s="10"/>
       <c r="F37" s="11"/>
       <c r="G37" s="10"/>
@@ -2176,7 +2908,7 @@
       <c r="O37" s="10"/>
       <c r="P37" s="10"/>
     </row>
-    <row r="38" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:21" ht="14.45" x14ac:dyDescent="0.35">
       <c r="E38" s="10"/>
       <c r="F38" s="11"/>
       <c r="G38" s="10"/>
@@ -2190,7 +2922,7 @@
       <c r="O38" s="10"/>
       <c r="P38" s="10"/>
     </row>
-    <row r="39" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:21" ht="14.45" x14ac:dyDescent="0.35">
       <c r="E39" s="10"/>
       <c r="F39" s="11"/>
       <c r="G39" s="10"/>
@@ -2204,7 +2936,7 @@
       <c r="O39" s="10"/>
       <c r="P39" s="10"/>
     </row>
-    <row r="40" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:21" ht="14.45" x14ac:dyDescent="0.35">
       <c r="E40" s="10"/>
       <c r="F40" s="11"/>
       <c r="G40" s="10"/>
@@ -2218,7 +2950,7 @@
       <c r="O40" s="10"/>
       <c r="P40" s="10"/>
     </row>
-    <row r="41" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:21" x14ac:dyDescent="0.25">
       <c r="E41" s="10"/>
       <c r="F41" s="11"/>
       <c r="G41" s="10"/>
@@ -2232,7 +2964,7 @@
       <c r="O41" s="10"/>
       <c r="P41" s="10"/>
     </row>
-    <row r="42" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:21" x14ac:dyDescent="0.25">
       <c r="E42" s="10"/>
       <c r="F42" s="11"/>
       <c r="G42" s="10"/>
@@ -2246,7 +2978,7 @@
       <c r="O42" s="10"/>
       <c r="P42" s="10"/>
     </row>
-    <row r="43" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:21" x14ac:dyDescent="0.25">
       <c r="E43" s="10"/>
       <c r="F43" s="11"/>
       <c r="G43" s="10"/>
@@ -2259,8 +2991,11 @@
       <c r="N43" s="10"/>
       <c r="O43" s="10"/>
       <c r="P43" s="10"/>
-    </row>
-    <row r="44" spans="5:16" x14ac:dyDescent="0.35">
+      <c r="T43" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="44" spans="2:21" x14ac:dyDescent="0.25">
       <c r="E44" s="10"/>
       <c r="F44" s="11"/>
       <c r="G44" s="10"/>
@@ -2273,8 +3008,15 @@
       <c r="N44" s="10"/>
       <c r="O44" s="10"/>
       <c r="P44" s="10"/>
-    </row>
-    <row r="45" spans="5:16" x14ac:dyDescent="0.35">
+      <c r="T44" t="s">
+        <v>34</v>
+      </c>
+      <c r="U44" s="32">
+        <f>COUNTIF(L2:L68,"*Minor*")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="2:21" x14ac:dyDescent="0.25">
       <c r="E45" s="10"/>
       <c r="F45" s="11"/>
       <c r="G45" s="10"/>
@@ -2287,8 +3029,15 @@
       <c r="N45" s="10"/>
       <c r="O45" s="10"/>
       <c r="P45" s="10"/>
-    </row>
-    <row r="46" spans="5:16" x14ac:dyDescent="0.35">
+      <c r="T45" t="s">
+        <v>57</v>
+      </c>
+      <c r="U45" s="32">
+        <f>COUNTIF(L2:L25,"*Moderate*")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="2:21" x14ac:dyDescent="0.25">
       <c r="E46" s="10"/>
       <c r="F46" s="11"/>
       <c r="G46" s="10"/>
@@ -2301,8 +3050,15 @@
       <c r="N46" s="10"/>
       <c r="O46" s="10"/>
       <c r="P46" s="10"/>
-    </row>
-    <row r="47" spans="5:16" x14ac:dyDescent="0.35">
+      <c r="T46" t="s">
+        <v>35</v>
+      </c>
+      <c r="U46" s="32">
+        <f>COUNTIF(L2:L25,"*Major*")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="2:21" x14ac:dyDescent="0.25">
       <c r="E47" s="10"/>
       <c r="F47" s="11"/>
       <c r="G47" s="10"/>
@@ -2315,8 +3071,15 @@
       <c r="N47" s="10"/>
       <c r="O47" s="10"/>
       <c r="P47" s="10"/>
-    </row>
-    <row r="48" spans="5:16" x14ac:dyDescent="0.35">
+      <c r="T47" t="s">
+        <v>36</v>
+      </c>
+      <c r="U47" s="32">
+        <f>COUNTIF(L2:L25,"*Critical*")</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="48" spans="2:21" x14ac:dyDescent="0.25">
       <c r="E48" s="10"/>
       <c r="F48" s="11"/>
       <c r="G48" s="10"/>
@@ -2329,8 +3092,15 @@
       <c r="N48" s="10"/>
       <c r="O48" s="10"/>
       <c r="P48" s="10"/>
-    </row>
-    <row r="49" spans="5:16" x14ac:dyDescent="0.35">
+      <c r="T48" t="s">
+        <v>38</v>
+      </c>
+      <c r="U48" s="32">
+        <f>COUNTIF(L2:L25,"*Cometic*")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E49" s="10"/>
       <c r="F49" s="11"/>
       <c r="G49" s="10"/>
@@ -2344,7 +3114,7 @@
       <c r="O49" s="10"/>
       <c r="P49" s="10"/>
     </row>
-    <row r="50" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="50" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E50" s="10"/>
       <c r="F50" s="11"/>
       <c r="G50" s="10"/>
@@ -2358,7 +3128,7 @@
       <c r="O50" s="10"/>
       <c r="P50" s="10"/>
     </row>
-    <row r="51" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="51" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E51" s="10"/>
       <c r="F51" s="11"/>
       <c r="G51" s="10"/>
@@ -2372,7 +3142,7 @@
       <c r="O51" s="10"/>
       <c r="P51" s="10"/>
     </row>
-    <row r="52" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="52" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E52" s="10"/>
       <c r="F52" s="11"/>
       <c r="G52" s="10"/>
@@ -2386,7 +3156,7 @@
       <c r="O52" s="10"/>
       <c r="P52" s="10"/>
     </row>
-    <row r="53" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="53" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E53" s="10"/>
       <c r="F53" s="11"/>
       <c r="G53" s="10"/>
@@ -2400,7 +3170,7 @@
       <c r="O53" s="10"/>
       <c r="P53" s="10"/>
     </row>
-    <row r="54" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="54" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E54" s="10"/>
       <c r="F54" s="11"/>
       <c r="G54" s="10"/>
@@ -2414,7 +3184,7 @@
       <c r="O54" s="10"/>
       <c r="P54" s="10"/>
     </row>
-    <row r="55" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="55" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E55" s="10"/>
       <c r="F55" s="11"/>
       <c r="G55" s="10"/>
@@ -2428,7 +3198,7 @@
       <c r="O55" s="10"/>
       <c r="P55" s="10"/>
     </row>
-    <row r="56" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="56" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E56" s="10"/>
       <c r="F56" s="11"/>
       <c r="G56" s="10"/>
@@ -2442,7 +3212,7 @@
       <c r="O56" s="10"/>
       <c r="P56" s="10"/>
     </row>
-    <row r="57" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="57" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E57" s="10"/>
       <c r="F57" s="11"/>
       <c r="G57" s="10"/>
@@ -2456,7 +3226,7 @@
       <c r="O57" s="10"/>
       <c r="P57" s="10"/>
     </row>
-    <row r="58" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="58" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E58" s="10"/>
       <c r="F58" s="11"/>
       <c r="G58" s="10"/>
@@ -2470,7 +3240,7 @@
       <c r="O58" s="10"/>
       <c r="P58" s="10"/>
     </row>
-    <row r="59" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="59" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E59" s="10"/>
       <c r="F59" s="11"/>
       <c r="G59" s="10"/>
@@ -2484,7 +3254,7 @@
       <c r="O59" s="10"/>
       <c r="P59" s="10"/>
     </row>
-    <row r="60" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="60" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E60" s="10"/>
       <c r="F60" s="11"/>
       <c r="G60" s="10"/>
@@ -2498,7 +3268,7 @@
       <c r="O60" s="10"/>
       <c r="P60" s="10"/>
     </row>
-    <row r="61" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="61" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E61" s="10"/>
       <c r="F61" s="11"/>
       <c r="G61" s="10"/>
@@ -2512,7 +3282,7 @@
       <c r="O61" s="10"/>
       <c r="P61" s="10"/>
     </row>
-    <row r="62" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="62" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E62" s="10"/>
       <c r="F62" s="11"/>
       <c r="G62" s="10"/>
@@ -2526,7 +3296,7 @@
       <c r="O62" s="10"/>
       <c r="P62" s="10"/>
     </row>
-    <row r="63" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="63" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E63" s="10"/>
       <c r="F63" s="11"/>
       <c r="G63" s="10"/>
@@ -2540,7 +3310,7 @@
       <c r="O63" s="10"/>
       <c r="P63" s="10"/>
     </row>
-    <row r="64" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="64" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E64" s="10"/>
       <c r="F64" s="11"/>
       <c r="G64" s="10"/>
@@ -2554,7 +3324,7 @@
       <c r="O64" s="10"/>
       <c r="P64" s="10"/>
     </row>
-    <row r="65" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="65" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E65" s="10"/>
       <c r="F65" s="11"/>
       <c r="G65" s="10"/>
@@ -2568,7 +3338,7 @@
       <c r="O65" s="10"/>
       <c r="P65" s="10"/>
     </row>
-    <row r="66" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="66" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E66" s="10"/>
       <c r="F66" s="11"/>
       <c r="G66" s="10"/>
@@ -2582,7 +3352,7 @@
       <c r="O66" s="10"/>
       <c r="P66" s="10"/>
     </row>
-    <row r="67" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="67" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E67" s="10"/>
       <c r="F67" s="11"/>
       <c r="G67" s="10"/>
@@ -2596,7 +3366,7 @@
       <c r="O67" s="10"/>
       <c r="P67" s="10"/>
     </row>
-    <row r="68" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="68" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E68" s="10"/>
       <c r="F68" s="11"/>
       <c r="G68" s="10"/>
@@ -2610,7 +3380,7 @@
       <c r="O68" s="10"/>
       <c r="P68" s="10"/>
     </row>
-    <row r="69" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="69" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E69" s="10"/>
       <c r="F69" s="11"/>
       <c r="G69" s="10"/>
@@ -2624,7 +3394,7 @@
       <c r="O69" s="10"/>
       <c r="P69" s="10"/>
     </row>
-    <row r="70" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="70" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E70" s="10"/>
       <c r="F70" s="11"/>
       <c r="G70" s="10"/>
@@ -2638,7 +3408,7 @@
       <c r="O70" s="10"/>
       <c r="P70" s="10"/>
     </row>
-    <row r="71" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="71" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E71" s="10"/>
       <c r="F71" s="11"/>
       <c r="G71" s="10"/>
@@ -2652,7 +3422,7 @@
       <c r="O71" s="10"/>
       <c r="P71" s="10"/>
     </row>
-    <row r="72" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="72" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E72" s="10"/>
       <c r="F72" s="11"/>
       <c r="G72" s="10"/>
@@ -2666,7 +3436,7 @@
       <c r="O72" s="10"/>
       <c r="P72" s="10"/>
     </row>
-    <row r="73" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="73" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E73" s="10"/>
       <c r="F73" s="11"/>
       <c r="G73" s="10"/>
@@ -2680,7 +3450,7 @@
       <c r="O73" s="10"/>
       <c r="P73" s="10"/>
     </row>
-    <row r="74" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="74" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E74" s="10"/>
       <c r="F74" s="11"/>
       <c r="G74" s="10"/>
@@ -2694,7 +3464,7 @@
       <c r="O74" s="10"/>
       <c r="P74" s="10"/>
     </row>
-    <row r="75" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="75" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E75" s="10"/>
       <c r="F75" s="11"/>
       <c r="G75" s="10"/>
@@ -2708,7 +3478,7 @@
       <c r="O75" s="10"/>
       <c r="P75" s="10"/>
     </row>
-    <row r="76" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="76" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E76" s="10"/>
       <c r="F76" s="11"/>
       <c r="G76" s="10"/>
@@ -2722,7 +3492,7 @@
       <c r="O76" s="10"/>
       <c r="P76" s="10"/>
     </row>
-    <row r="77" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="77" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E77" s="10"/>
       <c r="F77" s="11"/>
       <c r="G77" s="10"/>
@@ -2736,7 +3506,7 @@
       <c r="O77" s="10"/>
       <c r="P77" s="10"/>
     </row>
-    <row r="78" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="78" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E78" s="10"/>
       <c r="F78" s="11"/>
       <c r="G78" s="10"/>
@@ -2750,7 +3520,7 @@
       <c r="O78" s="10"/>
       <c r="P78" s="10"/>
     </row>
-    <row r="79" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="79" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E79" s="10"/>
       <c r="F79" s="11"/>
       <c r="G79" s="10"/>
@@ -2764,7 +3534,7 @@
       <c r="O79" s="10"/>
       <c r="P79" s="10"/>
     </row>
-    <row r="80" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="80" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E80" s="10"/>
       <c r="F80" s="11"/>
       <c r="G80" s="10"/>
@@ -2778,7 +3548,7 @@
       <c r="O80" s="10"/>
       <c r="P80" s="10"/>
     </row>
-    <row r="81" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="81" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E81" s="10"/>
       <c r="F81" s="11"/>
       <c r="G81" s="10"/>
@@ -2792,7 +3562,7 @@
       <c r="O81" s="10"/>
       <c r="P81" s="10"/>
     </row>
-    <row r="82" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="82" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E82" s="10"/>
       <c r="F82" s="11"/>
       <c r="G82" s="10"/>
@@ -2806,7 +3576,7 @@
       <c r="O82" s="10"/>
       <c r="P82" s="10"/>
     </row>
-    <row r="83" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="83" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E83" s="10"/>
       <c r="F83" s="11"/>
       <c r="G83" s="10"/>
@@ -2820,7 +3590,7 @@
       <c r="O83" s="10"/>
       <c r="P83" s="10"/>
     </row>
-    <row r="84" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="84" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E84" s="10"/>
       <c r="F84" s="11"/>
       <c r="G84" s="10"/>
@@ -2834,7 +3604,7 @@
       <c r="O84" s="10"/>
       <c r="P84" s="10"/>
     </row>
-    <row r="85" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="85" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E85" s="10"/>
       <c r="F85" s="11"/>
       <c r="G85" s="10"/>
@@ -2848,7 +3618,7 @@
       <c r="O85" s="10"/>
       <c r="P85" s="10"/>
     </row>
-    <row r="86" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="86" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E86" s="10"/>
       <c r="F86" s="11"/>
       <c r="G86" s="10"/>
@@ -2862,7 +3632,7 @@
       <c r="O86" s="10"/>
       <c r="P86" s="10"/>
     </row>
-    <row r="87" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="87" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E87" s="10"/>
       <c r="F87" s="11"/>
       <c r="G87" s="10"/>
@@ -2876,7 +3646,7 @@
       <c r="O87" s="10"/>
       <c r="P87" s="10"/>
     </row>
-    <row r="88" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="88" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E88" s="10"/>
       <c r="F88" s="11"/>
       <c r="G88" s="10"/>
@@ -2890,7 +3660,7 @@
       <c r="O88" s="10"/>
       <c r="P88" s="10"/>
     </row>
-    <row r="89" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="89" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E89" s="10"/>
       <c r="F89" s="11"/>
       <c r="G89" s="10"/>
@@ -2904,7 +3674,7 @@
       <c r="O89" s="10"/>
       <c r="P89" s="10"/>
     </row>
-    <row r="90" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="90" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E90" s="10"/>
       <c r="F90" s="11"/>
       <c r="G90" s="10"/>
@@ -2918,7 +3688,7 @@
       <c r="O90" s="10"/>
       <c r="P90" s="10"/>
     </row>
-    <row r="91" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="91" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E91" s="10"/>
       <c r="F91" s="11"/>
       <c r="G91" s="10"/>
@@ -2932,7 +3702,7 @@
       <c r="O91" s="10"/>
       <c r="P91" s="10"/>
     </row>
-    <row r="92" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="92" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E92" s="10"/>
       <c r="F92" s="11"/>
       <c r="G92" s="10"/>
@@ -2946,7 +3716,7 @@
       <c r="O92" s="10"/>
       <c r="P92" s="10"/>
     </row>
-    <row r="93" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="93" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E93" s="10"/>
       <c r="F93" s="11"/>
       <c r="G93" s="10"/>
@@ -2960,7 +3730,7 @@
       <c r="O93" s="10"/>
       <c r="P93" s="10"/>
     </row>
-    <row r="94" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="94" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E94" s="10"/>
       <c r="F94" s="11"/>
       <c r="G94" s="10"/>
@@ -2974,7 +3744,7 @@
       <c r="O94" s="10"/>
       <c r="P94" s="10"/>
     </row>
-    <row r="95" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="95" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E95" s="10"/>
       <c r="F95" s="11"/>
       <c r="G95" s="10"/>
@@ -2988,7 +3758,7 @@
       <c r="O95" s="10"/>
       <c r="P95" s="10"/>
     </row>
-    <row r="96" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="96" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E96" s="10"/>
       <c r="F96" s="11"/>
       <c r="G96" s="10"/>
@@ -3002,7 +3772,7 @@
       <c r="O96" s="10"/>
       <c r="P96" s="10"/>
     </row>
-    <row r="97" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="97" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E97" s="10"/>
       <c r="F97" s="11"/>
       <c r="G97" s="10"/>
@@ -3016,7 +3786,7 @@
       <c r="O97" s="10"/>
       <c r="P97" s="10"/>
     </row>
-    <row r="98" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="98" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E98" s="10"/>
       <c r="F98" s="11"/>
       <c r="G98" s="10"/>
@@ -3030,7 +3800,7 @@
       <c r="O98" s="10"/>
       <c r="P98" s="10"/>
     </row>
-    <row r="99" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="99" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E99" s="10"/>
       <c r="F99" s="11"/>
       <c r="G99" s="10"/>
@@ -3044,7 +3814,7 @@
       <c r="O99" s="10"/>
       <c r="P99" s="10"/>
     </row>
-    <row r="100" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="100" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E100" s="10"/>
       <c r="F100" s="11"/>
       <c r="G100" s="10"/>
@@ -3058,7 +3828,7 @@
       <c r="O100" s="10"/>
       <c r="P100" s="10"/>
     </row>
-    <row r="101" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="101" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E101" s="10"/>
       <c r="F101" s="11"/>
       <c r="G101" s="10"/>
@@ -3072,7 +3842,7 @@
       <c r="O101" s="10"/>
       <c r="P101" s="10"/>
     </row>
-    <row r="102" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="102" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E102" s="10"/>
       <c r="F102" s="11"/>
       <c r="G102" s="10"/>
@@ -3086,7 +3856,7 @@
       <c r="O102" s="10"/>
       <c r="P102" s="10"/>
     </row>
-    <row r="103" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="103" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E103" s="10"/>
       <c r="F103" s="11"/>
       <c r="G103" s="10"/>
@@ -3100,7 +3870,7 @@
       <c r="O103" s="10"/>
       <c r="P103" s="10"/>
     </row>
-    <row r="104" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="104" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E104" s="10"/>
       <c r="F104" s="11"/>
       <c r="G104" s="10"/>
@@ -3114,7 +3884,7 @@
       <c r="O104" s="10"/>
       <c r="P104" s="10"/>
     </row>
-    <row r="105" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="105" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E105" s="10"/>
       <c r="F105" s="11"/>
       <c r="G105" s="10"/>
@@ -3128,7 +3898,7 @@
       <c r="O105" s="10"/>
       <c r="P105" s="10"/>
     </row>
-    <row r="106" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="106" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E106" s="10"/>
       <c r="F106" s="11"/>
       <c r="G106" s="10"/>
@@ -3142,7 +3912,7 @@
       <c r="O106" s="10"/>
       <c r="P106" s="10"/>
     </row>
-    <row r="107" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="107" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E107" s="10"/>
       <c r="F107" s="11"/>
       <c r="G107" s="10"/>
@@ -3156,7 +3926,7 @@
       <c r="O107" s="10"/>
       <c r="P107" s="10"/>
     </row>
-    <row r="108" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="108" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E108" s="10"/>
       <c r="F108" s="11"/>
       <c r="G108" s="10"/>
@@ -3170,7 +3940,7 @@
       <c r="O108" s="10"/>
       <c r="P108" s="10"/>
     </row>
-    <row r="109" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="109" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E109" s="10"/>
       <c r="F109" s="11"/>
       <c r="G109" s="10"/>
@@ -3184,7 +3954,7 @@
       <c r="O109" s="10"/>
       <c r="P109" s="10"/>
     </row>
-    <row r="110" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="110" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E110" s="10"/>
       <c r="F110" s="11"/>
       <c r="G110" s="10"/>
@@ -3198,7 +3968,7 @@
       <c r="O110" s="10"/>
       <c r="P110" s="10"/>
     </row>
-    <row r="111" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="111" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E111" s="10"/>
       <c r="F111" s="11"/>
       <c r="G111" s="10"/>
@@ -3212,7 +3982,7 @@
       <c r="O111" s="10"/>
       <c r="P111" s="10"/>
     </row>
-    <row r="112" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="112" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E112" s="10"/>
       <c r="F112" s="11"/>
       <c r="G112" s="10"/>
@@ -3226,7 +3996,7 @@
       <c r="O112" s="10"/>
       <c r="P112" s="10"/>
     </row>
-    <row r="113" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="113" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E113" s="10"/>
       <c r="F113" s="11"/>
       <c r="G113" s="10"/>
@@ -3240,7 +4010,7 @@
       <c r="O113" s="10"/>
       <c r="P113" s="10"/>
     </row>
-    <row r="114" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="114" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E114" s="10"/>
       <c r="F114" s="11"/>
       <c r="G114" s="10"/>
@@ -3254,7 +4024,7 @@
       <c r="O114" s="10"/>
       <c r="P114" s="10"/>
     </row>
-    <row r="115" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="115" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E115" s="10"/>
       <c r="F115" s="11"/>
       <c r="G115" s="10"/>
@@ -3268,7 +4038,7 @@
       <c r="O115" s="10"/>
       <c r="P115" s="10"/>
     </row>
-    <row r="116" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="116" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E116" s="10"/>
       <c r="F116" s="11"/>
       <c r="G116" s="10"/>
@@ -3282,7 +4052,7 @@
       <c r="O116" s="10"/>
       <c r="P116" s="10"/>
     </row>
-    <row r="117" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="117" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E117" s="10"/>
       <c r="F117" s="11"/>
       <c r="G117" s="10"/>
@@ -3296,7 +4066,7 @@
       <c r="O117" s="10"/>
       <c r="P117" s="10"/>
     </row>
-    <row r="118" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="118" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E118" s="10"/>
       <c r="F118" s="11"/>
       <c r="G118" s="10"/>
@@ -3310,7 +4080,7 @@
       <c r="O118" s="10"/>
       <c r="P118" s="10"/>
     </row>
-    <row r="119" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="119" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E119" s="10"/>
       <c r="F119" s="11"/>
       <c r="G119" s="10"/>
@@ -3324,7 +4094,7 @@
       <c r="O119" s="10"/>
       <c r="P119" s="10"/>
     </row>
-    <row r="120" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="120" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E120" s="10"/>
       <c r="F120" s="11"/>
       <c r="G120" s="10"/>
@@ -3338,7 +4108,7 @@
       <c r="O120" s="10"/>
       <c r="P120" s="10"/>
     </row>
-    <row r="121" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="121" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E121" s="10"/>
       <c r="F121" s="11"/>
       <c r="G121" s="10"/>
@@ -3352,7 +4122,7 @@
       <c r="O121" s="10"/>
       <c r="P121" s="10"/>
     </row>
-    <row r="122" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="122" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E122" s="10"/>
       <c r="F122" s="11"/>
       <c r="G122" s="10"/>
@@ -3366,7 +4136,7 @@
       <c r="O122" s="10"/>
       <c r="P122" s="10"/>
     </row>
-    <row r="123" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="123" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E123" s="10"/>
       <c r="F123" s="11"/>
       <c r="G123" s="10"/>
@@ -3380,7 +4150,7 @@
       <c r="O123" s="10"/>
       <c r="P123" s="10"/>
     </row>
-    <row r="124" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="124" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E124" s="10"/>
       <c r="F124" s="11"/>
       <c r="G124" s="10"/>
@@ -3394,7 +4164,7 @@
       <c r="O124" s="10"/>
       <c r="P124" s="10"/>
     </row>
-    <row r="125" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="125" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E125" s="10"/>
       <c r="F125" s="11"/>
       <c r="G125" s="10"/>
@@ -3408,7 +4178,7 @@
       <c r="O125" s="10"/>
       <c r="P125" s="10"/>
     </row>
-    <row r="126" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="126" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E126" s="10"/>
       <c r="F126" s="11"/>
       <c r="G126" s="10"/>
@@ -3422,7 +4192,7 @@
       <c r="O126" s="10"/>
       <c r="P126" s="10"/>
     </row>
-    <row r="127" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="127" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E127" s="10"/>
       <c r="F127" s="11"/>
       <c r="G127" s="10"/>
@@ -3436,7 +4206,7 @@
       <c r="O127" s="10"/>
       <c r="P127" s="10"/>
     </row>
-    <row r="128" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="128" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E128" s="10"/>
       <c r="F128" s="11"/>
       <c r="G128" s="10"/>
@@ -3450,7 +4220,7 @@
       <c r="O128" s="10"/>
       <c r="P128" s="10"/>
     </row>
-    <row r="129" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="129" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E129" s="10"/>
       <c r="F129" s="11"/>
       <c r="G129" s="10"/>
@@ -3464,7 +4234,7 @@
       <c r="O129" s="10"/>
       <c r="P129" s="10"/>
     </row>
-    <row r="130" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="130" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E130" s="10"/>
       <c r="F130" s="11"/>
       <c r="G130" s="10"/>
@@ -3478,7 +4248,7 @@
       <c r="O130" s="10"/>
       <c r="P130" s="10"/>
     </row>
-    <row r="131" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="131" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E131" s="10"/>
       <c r="F131" s="11"/>
       <c r="G131" s="10"/>
@@ -3492,7 +4262,7 @@
       <c r="O131" s="10"/>
       <c r="P131" s="10"/>
     </row>
-    <row r="132" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="132" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E132" s="10"/>
       <c r="F132" s="11"/>
       <c r="G132" s="10"/>
@@ -3506,7 +4276,7 @@
       <c r="O132" s="10"/>
       <c r="P132" s="10"/>
     </row>
-    <row r="133" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="133" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E133" s="10"/>
       <c r="F133" s="11"/>
       <c r="G133" s="10"/>
@@ -3520,7 +4290,7 @@
       <c r="O133" s="10"/>
       <c r="P133" s="10"/>
     </row>
-    <row r="134" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="134" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E134" s="10"/>
       <c r="F134" s="11"/>
       <c r="G134" s="10"/>
@@ -3534,7 +4304,7 @@
       <c r="O134" s="10"/>
       <c r="P134" s="10"/>
     </row>
-    <row r="135" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="135" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E135" s="10"/>
       <c r="F135" s="11"/>
       <c r="G135" s="10"/>
@@ -3548,7 +4318,7 @@
       <c r="O135" s="10"/>
       <c r="P135" s="10"/>
     </row>
-    <row r="136" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="136" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E136" s="10"/>
       <c r="F136" s="11"/>
       <c r="G136" s="10"/>
@@ -3562,7 +4332,7 @@
       <c r="O136" s="10"/>
       <c r="P136" s="10"/>
     </row>
-    <row r="137" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="137" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E137" s="10"/>
       <c r="F137" s="11"/>
       <c r="G137" s="10"/>
@@ -3576,7 +4346,7 @@
       <c r="O137" s="10"/>
       <c r="P137" s="10"/>
     </row>
-    <row r="138" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="138" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E138" s="10"/>
       <c r="F138" s="11"/>
       <c r="G138" s="10"/>
@@ -3590,7 +4360,7 @@
       <c r="O138" s="10"/>
       <c r="P138" s="10"/>
     </row>
-    <row r="139" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="139" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E139" s="10"/>
       <c r="F139" s="11"/>
       <c r="G139" s="10"/>
@@ -3604,7 +4374,7 @@
       <c r="O139" s="10"/>
       <c r="P139" s="10"/>
     </row>
-    <row r="140" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="140" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E140" s="10"/>
       <c r="F140" s="11"/>
       <c r="G140" s="10"/>
@@ -3618,7 +4388,7 @@
       <c r="O140" s="10"/>
       <c r="P140" s="10"/>
     </row>
-    <row r="141" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="141" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E141" s="10"/>
       <c r="F141" s="11"/>
       <c r="G141" s="10"/>
@@ -3632,7 +4402,7 @@
       <c r="O141" s="10"/>
       <c r="P141" s="10"/>
     </row>
-    <row r="142" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="142" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E142" s="10"/>
       <c r="F142" s="11"/>
       <c r="G142" s="10"/>
@@ -3646,7 +4416,7 @@
       <c r="O142" s="10"/>
       <c r="P142" s="10"/>
     </row>
-    <row r="143" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="143" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E143" s="10"/>
       <c r="F143" s="11"/>
       <c r="G143" s="10"/>
@@ -3660,7 +4430,7 @@
       <c r="O143" s="10"/>
       <c r="P143" s="10"/>
     </row>
-    <row r="144" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="144" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E144" s="10"/>
       <c r="F144" s="11"/>
       <c r="G144" s="10"/>
@@ -3674,7 +4444,7 @@
       <c r="O144" s="10"/>
       <c r="P144" s="10"/>
     </row>
-    <row r="145" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="145" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E145" s="10"/>
       <c r="F145" s="11"/>
       <c r="G145" s="10"/>
@@ -3688,7 +4458,7 @@
       <c r="O145" s="10"/>
       <c r="P145" s="10"/>
     </row>
-    <row r="146" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="146" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E146" s="10"/>
       <c r="F146" s="11"/>
       <c r="G146" s="10"/>
@@ -3702,7 +4472,7 @@
       <c r="O146" s="10"/>
       <c r="P146" s="10"/>
     </row>
-    <row r="147" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="147" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E147" s="10"/>
       <c r="F147" s="11"/>
       <c r="G147" s="10"/>
@@ -3716,7 +4486,7 @@
       <c r="O147" s="10"/>
       <c r="P147" s="10"/>
     </row>
-    <row r="148" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="148" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E148" s="10"/>
       <c r="F148" s="11"/>
       <c r="G148" s="10"/>
@@ -3730,7 +4500,7 @@
       <c r="O148" s="10"/>
       <c r="P148" s="10"/>
     </row>
-    <row r="149" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="149" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E149" s="10"/>
       <c r="F149" s="11"/>
       <c r="G149" s="10"/>
@@ -3744,7 +4514,7 @@
       <c r="O149" s="10"/>
       <c r="P149" s="10"/>
     </row>
-    <row r="150" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="150" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E150" s="10"/>
       <c r="F150" s="11"/>
       <c r="G150" s="10"/>
@@ -3758,7 +4528,7 @@
       <c r="O150" s="10"/>
       <c r="P150" s="10"/>
     </row>
-    <row r="151" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="151" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E151" s="10"/>
       <c r="F151" s="11"/>
       <c r="G151" s="10"/>
@@ -3772,7 +4542,7 @@
       <c r="O151" s="10"/>
       <c r="P151" s="10"/>
     </row>
-    <row r="152" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="152" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E152" s="10"/>
       <c r="F152" s="11"/>
       <c r="G152" s="10"/>
@@ -3786,7 +4556,7 @@
       <c r="O152" s="10"/>
       <c r="P152" s="10"/>
     </row>
-    <row r="153" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="153" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E153" s="10"/>
       <c r="F153" s="11"/>
       <c r="G153" s="10"/>
@@ -3800,7 +4570,7 @@
       <c r="O153" s="10"/>
       <c r="P153" s="10"/>
     </row>
-    <row r="154" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="154" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E154" s="10"/>
       <c r="F154" s="11"/>
       <c r="G154" s="10"/>
@@ -3814,7 +4584,7 @@
       <c r="O154" s="10"/>
       <c r="P154" s="10"/>
     </row>
-    <row r="155" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="155" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E155" s="10"/>
       <c r="F155" s="11"/>
       <c r="G155" s="10"/>
@@ -3828,7 +4598,7 @@
       <c r="O155" s="10"/>
       <c r="P155" s="10"/>
     </row>
-    <row r="156" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="156" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E156" s="10"/>
       <c r="F156" s="11"/>
       <c r="G156" s="10"/>
@@ -3842,7 +4612,7 @@
       <c r="O156" s="10"/>
       <c r="P156" s="10"/>
     </row>
-    <row r="157" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="157" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E157" s="10"/>
       <c r="F157" s="11"/>
       <c r="G157" s="10"/>
@@ -3856,11 +4626,11 @@
       <c r="O157" s="10"/>
       <c r="P157" s="10"/>
     </row>
-    <row r="158" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="158" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E158" s="10"/>
       <c r="F158" s="11"/>
       <c r="G158" s="10"/>
-      <c r="H158" s="10"/>
+      <c r="H158" s="27"/>
       <c r="I158" s="10"/>
       <c r="J158" s="10"/>
       <c r="K158" s="10"/>
@@ -3870,11 +4640,11 @@
       <c r="O158" s="10"/>
       <c r="P158" s="10"/>
     </row>
-    <row r="159" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="159" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E159" s="10"/>
       <c r="F159" s="11"/>
       <c r="G159" s="10"/>
-      <c r="H159" s="10"/>
+      <c r="H159" s="27"/>
       <c r="I159" s="10"/>
       <c r="J159" s="10"/>
       <c r="K159" s="10"/>
@@ -3884,11 +4654,11 @@
       <c r="O159" s="10"/>
       <c r="P159" s="10"/>
     </row>
-    <row r="160" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="160" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E160" s="10"/>
-      <c r="F160" s="10"/>
+      <c r="F160" s="11"/>
       <c r="G160" s="10"/>
-      <c r="H160" s="10"/>
+      <c r="H160" s="27"/>
       <c r="I160" s="10"/>
       <c r="J160" s="10"/>
       <c r="K160" s="10"/>
@@ -3898,11 +4668,11 @@
       <c r="O160" s="10"/>
       <c r="P160" s="10"/>
     </row>
-    <row r="161" spans="5:16" x14ac:dyDescent="0.35">
+    <row r="161" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E161" s="10"/>
-      <c r="F161" s="10"/>
+      <c r="F161" s="11"/>
       <c r="G161" s="10"/>
-      <c r="H161" s="10"/>
+      <c r="H161" s="27"/>
       <c r="I161" s="10"/>
       <c r="J161" s="10"/>
       <c r="K161" s="10"/>
@@ -3912,10 +4682,262 @@
       <c r="O161" s="10"/>
       <c r="P161" s="10"/>
     </row>
+    <row r="162" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E162" s="10"/>
+      <c r="F162" s="11"/>
+      <c r="G162" s="10"/>
+      <c r="H162" s="27"/>
+      <c r="I162" s="10"/>
+      <c r="J162" s="10"/>
+      <c r="K162" s="10"/>
+      <c r="L162" s="10"/>
+      <c r="M162" s="10"/>
+      <c r="N162" s="10"/>
+      <c r="O162" s="10"/>
+      <c r="P162" s="10"/>
+    </row>
+    <row r="163" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E163" s="10"/>
+      <c r="F163" s="11"/>
+      <c r="G163" s="10"/>
+      <c r="H163" s="27"/>
+      <c r="I163" s="10"/>
+      <c r="J163" s="10"/>
+      <c r="K163" s="10"/>
+      <c r="L163" s="10"/>
+      <c r="M163" s="10"/>
+      <c r="N163" s="10"/>
+      <c r="O163" s="10"/>
+      <c r="P163" s="10"/>
+    </row>
+    <row r="164" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E164" s="10"/>
+      <c r="F164" s="11"/>
+      <c r="G164" s="10"/>
+      <c r="H164" s="27"/>
+      <c r="I164" s="10"/>
+      <c r="J164" s="10"/>
+      <c r="K164" s="10"/>
+      <c r="L164" s="10"/>
+      <c r="M164" s="10"/>
+      <c r="N164" s="10"/>
+      <c r="O164" s="10"/>
+      <c r="P164" s="10"/>
+    </row>
+    <row r="165" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E165" s="10"/>
+      <c r="F165" s="11"/>
+      <c r="G165" s="10"/>
+      <c r="H165" s="27"/>
+      <c r="I165" s="10"/>
+      <c r="J165" s="10"/>
+      <c r="K165" s="10"/>
+      <c r="L165" s="10"/>
+      <c r="M165" s="10"/>
+      <c r="N165" s="10"/>
+      <c r="O165" s="10"/>
+      <c r="P165" s="10"/>
+    </row>
+    <row r="166" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E166" s="10"/>
+      <c r="F166" s="11"/>
+      <c r="G166" s="10"/>
+      <c r="H166" s="27"/>
+      <c r="I166" s="10"/>
+      <c r="J166" s="10"/>
+      <c r="K166" s="10"/>
+      <c r="L166" s="10"/>
+      <c r="M166" s="10"/>
+      <c r="N166" s="10"/>
+      <c r="O166" s="10"/>
+      <c r="P166" s="10"/>
+    </row>
+    <row r="167" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E167" s="10"/>
+      <c r="F167" s="11"/>
+      <c r="G167" s="10"/>
+      <c r="H167" s="27"/>
+      <c r="I167" s="10"/>
+      <c r="J167" s="10"/>
+      <c r="K167" s="10"/>
+      <c r="L167" s="10"/>
+      <c r="M167" s="10"/>
+      <c r="N167" s="10"/>
+      <c r="O167" s="10"/>
+      <c r="P167" s="10"/>
+    </row>
+    <row r="168" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E168" s="10"/>
+      <c r="F168" s="11"/>
+      <c r="G168" s="10"/>
+      <c r="H168" s="27"/>
+      <c r="I168" s="10"/>
+      <c r="J168" s="10"/>
+      <c r="K168" s="10"/>
+      <c r="L168" s="10"/>
+      <c r="M168" s="10"/>
+      <c r="N168" s="10"/>
+      <c r="O168" s="10"/>
+      <c r="P168" s="10"/>
+    </row>
+    <row r="169" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E169" s="10"/>
+      <c r="F169" s="11"/>
+      <c r="G169" s="10"/>
+      <c r="H169" s="27"/>
+      <c r="I169" s="10"/>
+      <c r="J169" s="10"/>
+      <c r="K169" s="10"/>
+      <c r="L169" s="10"/>
+      <c r="M169" s="10"/>
+      <c r="N169" s="10"/>
+      <c r="O169" s="10"/>
+      <c r="P169" s="10"/>
+    </row>
+    <row r="170" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E170" s="10"/>
+      <c r="F170" s="11"/>
+      <c r="G170" s="10"/>
+      <c r="H170" s="27"/>
+      <c r="I170" s="10"/>
+      <c r="J170" s="10"/>
+      <c r="K170" s="10"/>
+      <c r="L170" s="10"/>
+      <c r="M170" s="10"/>
+      <c r="N170" s="10"/>
+      <c r="O170" s="10"/>
+      <c r="P170" s="10"/>
+    </row>
+    <row r="171" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E171" s="10"/>
+      <c r="F171" s="11"/>
+      <c r="G171" s="10"/>
+      <c r="H171" s="27"/>
+      <c r="I171" s="10"/>
+      <c r="J171" s="10"/>
+      <c r="K171" s="10"/>
+      <c r="L171" s="10"/>
+      <c r="M171" s="10"/>
+      <c r="N171" s="10"/>
+      <c r="O171" s="10"/>
+      <c r="P171" s="10"/>
+    </row>
+    <row r="172" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E172" s="10"/>
+      <c r="F172" s="11"/>
+      <c r="G172" s="10"/>
+      <c r="H172" s="27"/>
+      <c r="I172" s="10"/>
+      <c r="J172" s="10"/>
+      <c r="K172" s="10"/>
+      <c r="L172" s="10"/>
+      <c r="M172" s="10"/>
+      <c r="N172" s="10"/>
+      <c r="O172" s="10"/>
+      <c r="P172" s="10"/>
+    </row>
+    <row r="173" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E173" s="10"/>
+      <c r="F173" s="11"/>
+      <c r="G173" s="10"/>
+      <c r="H173" s="27"/>
+      <c r="I173" s="10"/>
+      <c r="J173" s="10"/>
+      <c r="K173" s="10"/>
+      <c r="L173" s="10"/>
+      <c r="M173" s="10"/>
+      <c r="N173" s="10"/>
+      <c r="O173" s="10"/>
+      <c r="P173" s="10"/>
+    </row>
+    <row r="174" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E174" s="10"/>
+      <c r="F174" s="11"/>
+      <c r="G174" s="10"/>
+      <c r="H174" s="27"/>
+      <c r="I174" s="10"/>
+      <c r="J174" s="10"/>
+      <c r="K174" s="10"/>
+      <c r="L174" s="10"/>
+      <c r="M174" s="10"/>
+      <c r="N174" s="10"/>
+      <c r="O174" s="10"/>
+      <c r="P174" s="10"/>
+    </row>
+    <row r="175" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E175" s="10"/>
+      <c r="F175" s="11"/>
+      <c r="G175" s="10"/>
+      <c r="H175" s="27"/>
+      <c r="I175" s="10"/>
+      <c r="J175" s="10"/>
+      <c r="K175" s="10"/>
+      <c r="L175" s="10"/>
+      <c r="M175" s="10"/>
+      <c r="N175" s="10"/>
+      <c r="O175" s="10"/>
+      <c r="P175" s="10"/>
+    </row>
+    <row r="176" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E176" s="10"/>
+      <c r="F176" s="11"/>
+      <c r="G176" s="10"/>
+      <c r="H176" s="10"/>
+      <c r="I176" s="10"/>
+      <c r="J176" s="10"/>
+      <c r="K176" s="10"/>
+      <c r="L176" s="10"/>
+      <c r="M176" s="10"/>
+      <c r="N176" s="10"/>
+      <c r="O176" s="10"/>
+      <c r="P176" s="10"/>
+    </row>
+    <row r="177" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E177" s="10"/>
+      <c r="F177" s="11"/>
+      <c r="G177" s="10"/>
+      <c r="H177" s="10"/>
+      <c r="I177" s="10"/>
+      <c r="J177" s="10"/>
+      <c r="K177" s="10"/>
+      <c r="L177" s="10"/>
+      <c r="M177" s="10"/>
+      <c r="N177" s="10"/>
+      <c r="O177" s="10"/>
+      <c r="P177" s="10"/>
+    </row>
+    <row r="178" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E178" s="10"/>
+      <c r="F178" s="10"/>
+      <c r="G178" s="10"/>
+      <c r="H178" s="10"/>
+      <c r="I178" s="10"/>
+      <c r="J178" s="10"/>
+      <c r="K178" s="10"/>
+      <c r="L178" s="10"/>
+      <c r="M178" s="10"/>
+      <c r="N178" s="10"/>
+      <c r="O178" s="10"/>
+      <c r="P178" s="10"/>
+    </row>
+    <row r="179" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E179" s="10"/>
+      <c r="F179" s="10"/>
+      <c r="G179" s="10"/>
+      <c r="H179" s="10"/>
+      <c r="I179" s="10"/>
+      <c r="J179" s="10"/>
+      <c r="K179" s="10"/>
+      <c r="L179" s="10"/>
+      <c r="M179" s="10"/>
+      <c r="N179" s="10"/>
+      <c r="O179" s="10"/>
+      <c r="P179" s="10"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="H44:H159">
+  <conditionalFormatting sqref="H62:H177">
     <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="Passed ">
-      <formula>NOT(ISERROR(SEARCH("Passed ",H44)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Passed ",H62)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3929,25 +4951,25 @@
           <x14:formula1>
             <xm:f>Settings!$A$4:$A$6</xm:f>
           </x14:formula1>
-          <xm:sqref>H2:H43</xm:sqref>
+          <xm:sqref>H2:H61</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Settings!$B$4:$B$6</xm:f>
           </x14:formula1>
-          <xm:sqref>F2:F159</xm:sqref>
+          <xm:sqref>F2:F177</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Settings!$F$4:$F$8</xm:f>
           </x14:formula1>
-          <xm:sqref>L2:L7</xm:sqref>
+          <xm:sqref>L2:L25</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Settings!$D$4:$D$6</xm:f>
           </x14:formula1>
-          <xm:sqref>K2:K11</xm:sqref>
+          <xm:sqref>K2:K29</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -3963,21 +4985,20 @@
   <dimension ref="A1:M19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="15.6328125" customWidth="1"/>
-    <col min="3" max="3" width="35.26953125" customWidth="1"/>
-    <col min="4" max="5" width="24.1796875" customWidth="1"/>
-    <col min="6" max="6" width="18.6328125" customWidth="1"/>
-    <col min="7" max="7" width="14.6328125" customWidth="1"/>
-    <col min="8" max="8" width="13.1796875" customWidth="1"/>
-    <col min="9" max="9" width="13.08984375" customWidth="1"/>
+    <col min="1" max="2" width="15.5703125" customWidth="1"/>
+    <col min="3" max="3" width="35.28515625" customWidth="1"/>
+    <col min="4" max="5" width="24.140625" customWidth="1"/>
+    <col min="6" max="6" width="18.5703125" customWidth="1"/>
+    <col min="7" max="7" width="14.5703125" customWidth="1"/>
+    <col min="8" max="9" width="13.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" ht="29.1" x14ac:dyDescent="0.35">
       <c r="A1" s="21" t="s">
         <v>13</v>
       </c>
@@ -4003,12 +5024,22 @@
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
     </row>
-    <row r="2" spans="1:13" ht="23.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
+    <row r="2" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>136</v>
+      </c>
       <c r="F2" s="1"/>
       <c r="H2" s="28" t="s">
         <v>52</v>
@@ -4019,12 +5050,22 @@
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
+    <row r="3" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>136</v>
+      </c>
       <c r="F3" s="2"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
@@ -4034,12 +5075,22 @@
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
+    <row r="4" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C4" s="33" t="s">
+        <v>143</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>136</v>
+      </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
@@ -4049,12 +5100,22 @@
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
+    <row r="5" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>136</v>
+      </c>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
@@ -4064,12 +5125,22 @@
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
+    <row r="6" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>136</v>
+      </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
@@ -4079,12 +5150,22 @@
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
+    <row r="7" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>136</v>
+      </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
@@ -4094,12 +5175,22 @@
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
+    <row r="8" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>136</v>
+      </c>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
@@ -4109,12 +5200,22 @@
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
+    <row r="9" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>136</v>
+      </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
@@ -4124,12 +5225,22 @@
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
+    <row r="10" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>136</v>
+      </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
@@ -4139,12 +5250,22 @@
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
+    <row r="11" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>136</v>
+      </c>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
@@ -4154,12 +5275,22 @@
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
+    <row r="12" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>136</v>
+      </c>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
@@ -4169,12 +5300,22 @@
       <c r="L12" s="1"/>
       <c r="M12" s="1"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
+    <row r="13" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>136</v>
+      </c>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
@@ -4184,12 +5325,22 @@
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
+    <row r="14" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>136</v>
+      </c>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
@@ -4199,12 +5350,14 @@
       <c r="L14" s="1"/>
       <c r="M14" s="1"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
+      <c r="E15" s="1" t="s">
+        <v>137</v>
+      </c>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
@@ -4214,7 +5367,7 @@
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:13" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -4229,7 +5382,7 @@
       <c r="L16" s="1"/>
       <c r="M16" s="1"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:13" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -4244,7 +5397,7 @@
       <c r="L17" s="1"/>
       <c r="M17" s="1"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:13" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -4259,7 +5412,7 @@
       <c r="L18" s="1"/>
       <c r="M18" s="1"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:13" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -4287,11 +5440,11 @@
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.36328125" customWidth="1"/>
-    <col min="2" max="2" width="14.36328125" customWidth="1"/>
-    <col min="6" max="6" width="14.453125" customWidth="1"/>
+    <col min="1" max="1" width="17.42578125" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
@@ -4495,13 +5648,34 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{64745CD4-DB27-427B-80D9-1CCB91D6E4BC}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{64745CD4-DB27-427B-80D9-1CCB91D6E4BC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A346E62E-1A2C-4E03-B91F-FE4FC47F8E89}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A346E62E-1A2C-4E03-B91F-FE4FC47F8E89}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FEF49AB9-68C3-4E70-84F5-930D4AF0373D}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FEF49AB9-68C3-4E70-84F5-930D4AF0373D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>